<commit_message>
generate excel file with styles and datas
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -26,6 +26,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
+    <t xml:space="preserve">nome_fantasia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">razao_social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnpj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endereco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bairro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cidade</t>
+  </si>
+  <si>
     <t xml:space="preserve">Empresa 1</t>
   </si>
   <si>
@@ -123,6 +144,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
+    <font/>
   </fonts>
   <fills>
     <fill>
@@ -131,8 +159,92 @@
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -146,6 +258,13 @@
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="3" fillId="4" borderId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="4" fillId="5" borderId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="5" fillId="6" borderId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="6" fillId="7" borderId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="7" fillId="8" borderId="7" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,25 +552,25 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="4">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="7">
         <v>6</v>
       </c>
     </row>
@@ -522,6 +641,29 @@
       </c>
       <c r="G4" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>